<commit_message>
Latest code for ci/cd
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/Add_Supplier_Afghanistan.xlsx
+++ b/src/test/resources/test-data/Add_Supplier_Afghanistan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowWidth="17028" windowHeight="7944"/>
   </bookViews>
   <sheets>
     <sheet name="Add_Supplier" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Sheet1" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <oleSize ref="A1:I12"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="60">
   <si>
     <t>Company_Name</t>
   </si>
@@ -61,67 +62,67 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Dailyregress01</t>
-  </si>
-  <si>
-    <t>Dailyregress01@yopmail.com</t>
+    <t>supplierregress01</t>
+  </si>
+  <si>
+    <t>supplierregress01@yopmail.com</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
+    <t>supplierregress02</t>
+  </si>
+  <si>
+    <t>supplierregress02@yopmail.com</t>
+  </si>
+  <si>
+    <t>supplierregress03</t>
+  </si>
+  <si>
+    <t>supplierregress03@yopmail.com</t>
+  </si>
+  <si>
+    <t>supplierregress04</t>
+  </si>
+  <si>
+    <t>supplierregress04@yopmail.com</t>
+  </si>
+  <si>
+    <t>supplierregress05</t>
+  </si>
+  <si>
+    <t>supplierregress05@yopmail.com</t>
+  </si>
+  <si>
+    <t>supplierregress06</t>
+  </si>
+  <si>
+    <t>supplierregress06@yopmail.com</t>
+  </si>
+  <si>
+    <t>supplierregress07</t>
+  </si>
+  <si>
+    <t>supplierregress07@yopmail.com</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Currenturl</t>
+  </si>
+  <si>
+    <t>CocCurrentUrl</t>
+  </si>
+  <si>
     <t>Dailyregress02</t>
   </si>
   <si>
     <t>Dailyregress02@yopmail.com</t>
   </si>
   <si>
-    <t>Dailyregress03</t>
-  </si>
-  <si>
-    <t>Dailyregress03@yopmail.com</t>
-  </si>
-  <si>
-    <t>Dailyregress04</t>
-  </si>
-  <si>
-    <t>Dailyregress04@yopmail.com</t>
-  </si>
-  <si>
-    <t>Dailyregress05</t>
-  </si>
-  <si>
-    <t>Dailyregress05@yopmail.com</t>
-  </si>
-  <si>
-    <t>Dailyregress06</t>
-  </si>
-  <si>
-    <t>Dailyregress06@yopmail.com</t>
-  </si>
-  <si>
-    <t>Dailyregress07</t>
-  </si>
-  <si>
-    <t>Dailyregress07@yopmail.com</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Currenturl</t>
-  </si>
-  <si>
-    <t>CocCurrentUrl</t>
-  </si>
-  <si>
-    <t>Regressauto001</t>
-  </si>
-  <si>
-    <t>Regressauto001@yopmail.com</t>
-  </si>
-  <si>
-    <t>https://qa.daato.app/requests/680884d5983bed769dea60c9/main</t>
+    <t>https://qa.daato.app/requests/6809cc8e983bed769dede565/main</t>
   </si>
   <si>
     <t>Categories</t>
@@ -212,12 +213,6 @@
   </si>
   <si>
     <t>Responsible Sourcing</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>https://qa.daato.app/requests/6809cc8e983bed769dede565/main</t>
   </si>
 </sst>
 </file>
@@ -1219,23 +1214,23 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.1111111111111" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="38.4444444444444" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="9" width="26.3333333333333" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="19.4444444444444" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.1111111111111" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.46484375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="15.8046875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.6666666666667" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="10.3333333333333" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.7777777777778" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="13.4444444444444" collapsed="true"/>
+    <col min="1" max="1" width="27.1111111111111" customWidth="1"/>
+    <col min="2" max="2" width="38.4444444444444" customWidth="1"/>
+    <col min="3" max="3" width="26.3333333333333" style="9" customWidth="1"/>
+    <col min="4" max="4" width="19.4444444444444" customWidth="1"/>
+    <col min="5" max="5" width="19.1111111111111" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="12.462962962963" customWidth="1"/>
+    <col min="8" max="8" width="15.8055555555556" customWidth="1"/>
+    <col min="9" max="9" width="14.6666666666667" customWidth="1"/>
+    <col min="10" max="10" width="10.3333333333333" customWidth="1"/>
+    <col min="11" max="11" width="14.7777777777778" customWidth="1"/>
+    <col min="12" max="12" width="13.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:9">
@@ -1287,10 +1282,10 @@
         <v>35</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="I2">
         <v>12</v>
@@ -1316,7 +1311,7 @@
         <v>35</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>11</v>
@@ -1478,13 +1473,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="Dailyregress02@yopmail.com" tooltip="mailto:Dailyregress01@yopmail.com"/>
-    <hyperlink ref="B4" r:id="rId1" display="Dailyregress03@yopmail.com" tooltip="mailto:Dailyregress01@yopmail.com"/>
-    <hyperlink ref="B5" r:id="rId1" display="Dailyregress04@yopmail.com" tooltip="mailto:Dailyregress01@yopmail.com"/>
-    <hyperlink ref="B6" r:id="rId1" display="Dailyregress05@yopmail.com" tooltip="mailto:Dailyregress01@yopmail.com"/>
-    <hyperlink ref="B7" r:id="rId1" display="Dailyregress06@yopmail.com" tooltip="mailto:Dailyregress01@yopmail.com"/>
-    <hyperlink ref="B8" r:id="rId1" display="Dailyregress07@yopmail.com" tooltip="mailto:Dailyregress01@yopmail.com"/>
-    <hyperlink ref="B2" r:id="rId1" display="Dailyregress01@yopmail.com" tooltip="mailto:Dailyregress01@yopmail.com"/>
+    <hyperlink ref="B3" r:id="rId1" display="supplierregress02@yopmail.com" tooltip="mailto:supplierregress01@yopmail.com"/>
+    <hyperlink ref="B4" r:id="rId1" display="supplierregress03@yopmail.com" tooltip="mailto:supplierregress01@yopmail.com"/>
+    <hyperlink ref="B5" r:id="rId1" display="supplierregress04@yopmail.com" tooltip="mailto:supplierregress01@yopmail.com"/>
+    <hyperlink ref="B6" r:id="rId1" display="supplierregress05@yopmail.com" tooltip="mailto:supplierregress01@yopmail.com"/>
+    <hyperlink ref="B7" r:id="rId1" display="supplierregress06@yopmail.com" tooltip="mailto:supplierregress01@yopmail.com"/>
+    <hyperlink ref="B8" r:id="rId1" display="supplierregress07@yopmail.com" tooltip="mailto:supplierregress01@yopmail.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="supplierregress01@yopmail.com" tooltip="mailto:supplierregress01@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -1502,11 +1497,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.91015625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.7421875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="61.203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="63.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="46.0" collapsed="true"/>
+    <col min="1" max="1" width="15.9074074074074" customWidth="1"/>
+    <col min="2" max="2" width="27.7407407407407" customWidth="1"/>
+    <col min="3" max="3" width="61.2037037037037" customWidth="1"/>
+    <col min="4" max="4" width="63" customWidth="1"/>
+    <col min="5" max="5" width="46" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1526,13 +1521,13 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="3:3">
@@ -1540,7 +1535,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Regressauto001@yopmail.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="Dailyregress02@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1558,14 +1553,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="48.1111111111111" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="44.51171875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="43.4444444444444" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.8888888888889" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="35.12890625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="25.5555555555556" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="35.23046875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="23.4444444444444" collapsed="true"/>
+    <col min="1" max="1" width="48.1111111111111" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="44.5092592592593" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="43.4444444444444" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.8888888888889" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.1296296296296" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="25.5555555555556" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="35.2314814814815" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="23.4444444444444" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1853,11 +1848,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.2222222222222" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.3425925925926" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="20.5555555555556" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="23.83984375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="28.1111111111111" collapsed="true"/>
+    <col min="1" max="1" width="34.2222222222222" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.3425925925926" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.5555555555556" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.8425925925926" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.1111111111111" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2115,9 +2110,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.91015625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="27.7421875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.4444444444444" collapsed="true"/>
+    <col min="1" max="1" width="15.9074074074074" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.7407407407407" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.4444444444444" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2135,10 +2130,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C2">
         <v>12</v>

</xml_diff>